<commit_message>
started to add sheet links
</commit_message>
<xml_diff>
--- a/mitmh_2022_puzz_info.xlsx
+++ b/mitmh_2022_puzz_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/Puzzles/web_tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/Puzzles/web_tracker/DavidBerardo.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA06C7EF-1FC7-DF49-9308-47945671BD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1AE551-B14B-6A4B-AD51-DB715CF1635F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="840" windowWidth="21640" windowHeight="18460" xr2:uid="{18C2E303-1B2D-4829-A982-F09375C4C5EF}"/>
+    <workbookView xWindow="28640" yWindow="1920" windowWidth="21640" windowHeight="18460" xr2:uid="{18C2E303-1B2D-4829-A982-F09375C4C5EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="178">
   <si>
     <t>Round</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Solution</t>
   </si>
   <si>
-    <t>Meta: The Investigation</t>
-  </si>
-  <si>
     <t>https://www.bookspace.world/puzzle/ada-twist-scientist/</t>
   </si>
   <si>
@@ -333,27 +330,6 @@
     <t>https://docs.google.com/spreadsheets/d/1z9P53rlDnan3ItgU1EzhHEynFhD-tOM3Xi6_sFutIKY/edit#gid=0</t>
   </si>
   <si>
-    <t>Meta: Fruit Around</t>
-  </si>
-  <si>
-    <t>Meta: The Ministry</t>
-  </si>
-  <si>
-    <t>Meta: Billie Barker</t>
-  </si>
-  <si>
-    <t>Meta: Danni Dewey</t>
-  </si>
-  <si>
-    <t>Meta: Herschel Hayden</t>
-  </si>
-  <si>
-    <t>Meta: Alexei Lewis</t>
-  </si>
-  <si>
-    <t>Meta: Randy and Riley Rotch</t>
-  </si>
-  <si>
     <t>Crooked Crossings</t>
   </si>
   <si>
@@ -447,9 +423,6 @@
     <t>What's in the Box? What's in the Box?</t>
   </si>
   <si>
-    <t>Meta: The Case of the Missing Component</t>
-  </si>
-  <si>
     <t>https://www.bookspace.world/puzzle/the-case-of-the-missing-component/</t>
   </si>
   <si>
@@ -532,6 +505,69 @@
   </si>
   <si>
     <t>Pen Station</t>
+  </si>
+  <si>
+    <t>Fruit Around</t>
+  </si>
+  <si>
+    <t>Billie Barker</t>
+  </si>
+  <si>
+    <t>Danni Dewey</t>
+  </si>
+  <si>
+    <t>Herschel Hayden</t>
+  </si>
+  <si>
+    <t>Alexei Lewis</t>
+  </si>
+  <si>
+    <t>Randy and Riley Rotch</t>
+  </si>
+  <si>
+    <t>The Case of the Missing Component</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1zDao06Z3CPeS8cnND3XpPDKI_tYqHVPEQ6VS-41sCFk/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1OkfX8VGeFt7UvigCXBhdRR1mH4tC6-NNnX_nLtxp_CM/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/13GbKKnXw-JdwQLFqn8yqK2MVrVMmgOMMcnMqLlnf9NA/edit?usp=sharing,</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/13aF3gezwb0qaYReaK_SdKDq7XapKZ-d0sfTjBFviU-g/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/15OxP3eJhyeqYnylHNL0YoqvEaakgOhaGQruZKePJQJ0/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/spreadsheets/d/16TDmwqgtUHpZ2xsGrYMUx8NTtHrPqOk-09v4Xln-oac/edit?usp=sharing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1Pi0A2G50Lr4eL2_gt1BAv8PNBXrqKGz3AJNg2ei5shQ/edit?usp=sharing </t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1TM1wquMH_mukseOxIzj7Uvird_4bx20A53PlxzP9Ul4/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1ZgXKBDJt-enhBZUElzJ5fPUbTyRYSFmLVgyZy0PEuIw/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1gaI3hSed6JfvIjwRZpmfq2OlfahTzKOb2BQOCDdrKks/edit?usp=sharing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1iw-AQk6X6aCyyaYlLyieklvrImo2DAT8L03AQxBx_TE/edit?usp=sharing </t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1qKqg4VL6S4NvdCp83hpxoIF46SrbH2jAXKTJe12P_jI/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1w0LK7K59jo1Z_V8iWVDaFirkfNjbCQ8vyD1xafyQ_Tc/edit?usp=sharing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1xfeSllCgDn41VYTMsJds95PJa9umaxWKB5tAtvOkoNg/edit?usp=sharing </t>
   </si>
 </sst>
 </file>
@@ -912,15 +948,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554942BF-2343-48E3-ABF4-418BC56A8D3C}">
   <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I184"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -952,13 +988,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -975,16 +1011,16 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -998,10 +1034,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1018,16 +1054,16 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1041,16 +1077,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1064,10 +1100,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1084,16 +1120,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1107,16 +1143,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1130,16 +1166,16 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1153,10 +1189,10 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1173,16 +1209,16 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1190,13 +1226,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1207,13 +1243,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1224,16 +1260,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1244,13 +1280,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1261,13 +1297,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1278,16 +1314,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1298,16 +1334,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1318,10 +1354,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="str">
         <f>CONCATENATE("https://www.bookspace.world/puzzle/",SUBSTITUTE(LOWER(B20)," ","-"),"/")</f>
@@ -1336,10 +1372,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" ref="C21:C84" si="0">CONCATENATE("https://www.bookspace.world/puzzle/",SUBSTITUTE(LOWER(B21)," ","-"),"/")</f>
@@ -1354,13 +1390,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1371,13 +1407,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1388,13 +1424,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1405,10 +1441,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -1423,10 +1459,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -1441,13 +1477,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1458,13 +1494,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1475,10 +1511,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -1493,10 +1529,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -1511,10 +1547,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -1529,10 +1565,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -1547,10 +1583,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -1565,10 +1601,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -1583,10 +1619,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -1601,13 +1637,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1618,10 +1654,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -1636,10 +1672,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -1654,23 +1690,23 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/make-way-for-ducklings/</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -1678,17 +1714,17 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/the-talking-tree/</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1699,22 +1735,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E41">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1722,10 +1758,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -1740,23 +1776,23 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/crewel/</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E43">
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1764,16 +1800,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1784,13 +1820,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>129</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1801,14 +1840,17 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/crooked-crossings/</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1819,14 +1861,17 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/curious-and-determined/</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1837,14 +1882,17 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/dancing-triangles/</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -1855,14 +1903,17 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/the-downtown-murders/</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1873,14 +1924,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/the-hound-of-the-vast-cur-villes/</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -1891,13 +1945,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1908,14 +1965,17 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/mysterious-mechanics/</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1926,14 +1986,17 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/once-is-happenstance/</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1944,14 +2007,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/please-prove-you-are-human/</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1962,14 +2028,17 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/sparksnotes/</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1980,14 +2049,17 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/strange-garnets/</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1998,14 +2070,17 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/the-thin-pan/</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -2016,14 +2091,17 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
         <v>https://www.bookspace.world/puzzle/trickster-tales/</v>
+      </c>
+      <c r="D58" t="s">
+        <v>164</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -2034,13 +2112,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -2051,10 +2129,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -2069,10 +2147,10 @@
     </row>
     <row r="61" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -2087,10 +2165,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -2105,10 +2183,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -2123,10 +2201,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -2141,10 +2219,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -2159,10 +2237,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -2177,10 +2255,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="0"/>
@@ -2195,10 +2273,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="0"/>
@@ -2213,10 +2291,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="0"/>
@@ -2231,13 +2309,13 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C70" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -2248,13 +2326,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" t="s">
         <v>132</v>
-      </c>
-      <c r="C71" t="s">
-        <v>141</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -2265,10 +2343,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="0"/>
@@ -2283,10 +2361,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="0"/>
@@ -2301,10 +2379,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B74" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="0"/>
@@ -2319,13 +2397,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B75" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C75" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -2336,13 +2414,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B76" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" t="s">
         <v>144</v>
-      </c>
-      <c r="C76" t="s">
-        <v>153</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -2353,10 +2431,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="0"/>
@@ -2371,10 +2449,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="0"/>
@@ -2389,10 +2467,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B79" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="0"/>
@@ -2407,10 +2485,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="0"/>
@@ -2425,10 +2503,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="0"/>
@@ -2443,10 +2521,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="0"/>
@@ -2461,10 +2539,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="0"/>
@@ -2479,10 +2557,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B84" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="0"/>
@@ -2497,7 +2575,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" ref="C85:C148" si="1">CONCATENATE("https://www.bookspace.world/puzzle/",SUBSTITUTE(LOWER(B85)," ","-"),"/")</f>
@@ -2509,7 +2587,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -2521,7 +2599,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -2533,7 +2611,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
@@ -2545,7 +2623,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
@@ -2557,7 +2635,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
@@ -2569,7 +2647,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
@@ -2581,7 +2659,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
@@ -2593,7 +2671,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
@@ -2605,7 +2683,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
@@ -2617,7 +2695,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
@@ -2629,7 +2707,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
@@ -2641,7 +2719,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
@@ -2653,7 +2731,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
@@ -2665,7 +2743,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
@@ -2677,7 +2755,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
@@ -2689,7 +2767,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
@@ -2701,7 +2779,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
@@ -2713,7 +2791,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
@@ -2725,7 +2803,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
@@ -2737,7 +2815,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
@@ -2749,7 +2827,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
@@ -2761,7 +2839,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
@@ -2773,7 +2851,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
@@ -2785,7 +2863,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
@@ -2797,7 +2875,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
@@ -2809,7 +2887,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
@@ -2821,7 +2899,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
@@ -2833,7 +2911,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
@@ -2845,7 +2923,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
@@ -2857,7 +2935,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
@@ -2869,7 +2947,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
@@ -2881,7 +2959,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
@@ -2893,7 +2971,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
@@ -2905,7 +2983,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
@@ -2917,7 +2995,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
@@ -2929,7 +3007,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
@@ -2941,7 +3019,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
@@ -2953,7 +3031,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
@@ -2965,7 +3043,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
@@ -2977,7 +3055,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
@@ -2989,7 +3067,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
@@ -3001,7 +3079,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="1"/>
@@ -3013,7 +3091,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="1"/>
@@ -3025,7 +3103,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="1"/>
@@ -3037,7 +3115,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="1"/>
@@ -3049,7 +3127,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" si="1"/>
@@ -3061,7 +3139,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="1"/>
@@ -3073,7 +3151,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="1"/>
@@ -3085,7 +3163,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="1"/>
@@ -3097,7 +3175,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="1"/>
@@ -3109,7 +3187,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="1"/>
@@ -3121,7 +3199,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="1"/>
@@ -3133,7 +3211,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="1"/>
@@ -3145,7 +3223,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="1"/>
@@ -3157,7 +3235,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C140" t="str">
         <f t="shared" si="1"/>
@@ -3169,7 +3247,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C141" t="str">
         <f t="shared" si="1"/>
@@ -3181,7 +3259,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C142" t="str">
         <f t="shared" si="1"/>
@@ -3193,7 +3271,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C143" t="str">
         <f t="shared" si="1"/>
@@ -3205,7 +3283,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C144" t="str">
         <f t="shared" si="1"/>
@@ -3217,7 +3295,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C145" t="str">
         <f t="shared" si="1"/>
@@ -3229,7 +3307,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C146" t="str">
         <f t="shared" si="1"/>
@@ -3241,7 +3319,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C147" t="str">
         <f t="shared" si="1"/>
@@ -3253,7 +3331,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C148" t="str">
         <f t="shared" si="1"/>
@@ -3265,7 +3343,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C149" t="str">
         <f t="shared" ref="C149:C183" si="2">CONCATENATE("https://www.bookspace.world/puzzle/",SUBSTITUTE(LOWER(B149)," ","-"),"/")</f>
@@ -3277,7 +3355,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C150" t="str">
         <f t="shared" si="2"/>
@@ -3289,7 +3367,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C151" t="str">
         <f t="shared" si="2"/>
@@ -3301,7 +3379,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C152" t="str">
         <f t="shared" si="2"/>
@@ -3313,7 +3391,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="2"/>
@@ -3325,7 +3403,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="2"/>
@@ -3337,7 +3415,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C155" t="str">
         <f t="shared" si="2"/>
@@ -3349,7 +3427,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C156" t="str">
         <f t="shared" si="2"/>
@@ -3361,7 +3439,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C157" t="str">
         <f t="shared" si="2"/>
@@ -3373,7 +3451,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C158" t="str">
         <f t="shared" si="2"/>
@@ -3385,7 +3463,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C159" t="str">
         <f t="shared" si="2"/>
@@ -3397,7 +3475,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C160" t="str">
         <f t="shared" si="2"/>
@@ -3409,7 +3487,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C161" t="str">
         <f t="shared" si="2"/>
@@ -3421,7 +3499,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C162" t="str">
         <f t="shared" si="2"/>
@@ -3433,7 +3511,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="2"/>
@@ -3445,7 +3523,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C164" t="str">
         <f t="shared" si="2"/>
@@ -3457,7 +3535,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C165" t="str">
         <f t="shared" si="2"/>
@@ -3469,7 +3547,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C166" t="str">
         <f t="shared" si="2"/>
@@ -3481,7 +3559,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C167" t="str">
         <f t="shared" si="2"/>
@@ -3493,7 +3571,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C168" t="str">
         <f t="shared" si="2"/>
@@ -3505,7 +3583,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C169" t="str">
         <f t="shared" si="2"/>
@@ -3517,7 +3595,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="2"/>
@@ -3529,7 +3607,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C171" t="str">
         <f t="shared" si="2"/>
@@ -3541,7 +3619,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C172" t="str">
         <f t="shared" si="2"/>
@@ -3553,7 +3631,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C173" t="str">
         <f t="shared" si="2"/>
@@ -3565,7 +3643,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C174" t="str">
         <f t="shared" si="2"/>
@@ -3577,7 +3655,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C175" t="str">
         <f t="shared" si="2"/>
@@ -3589,7 +3667,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C176" t="str">
         <f t="shared" si="2"/>
@@ -3601,7 +3679,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C177" t="str">
         <f t="shared" si="2"/>
@@ -3613,7 +3691,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C178" t="str">
         <f t="shared" si="2"/>
@@ -3625,7 +3703,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C179" t="str">
         <f t="shared" si="2"/>
@@ -3637,7 +3715,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C180" t="str">
         <f t="shared" si="2"/>
@@ -3649,7 +3727,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C181" t="str">
         <f t="shared" si="2"/>
@@ -3661,7 +3739,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C182" t="str">
         <f t="shared" si="2"/>
@@ -3673,7 +3751,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C183" t="str">
         <f t="shared" si="2"/>
@@ -3696,8 +3774,21 @@
     <hyperlink ref="D10" r:id="rId9" location="gid=0" display="https://docs.google.com/spreadsheets/d/1VjcDHkGBvZt6l8ltYiWhbQEfWRYRh9R5UBKjPoF52gg/edit - gid=0" xr:uid="{598B8B09-291D-460E-AC83-E026CABEF6C1}"/>
     <hyperlink ref="D8" r:id="rId10" location="gid=0" display="https://docs.google.com/spreadsheets/d/1wX8v0WCEHUABBnaZ_eneAbtaW5nqddNZjsdtT7xSdoY/edit - gid=0" xr:uid="{B3BFC9CE-ED57-4117-A107-FC337DAD9318}"/>
     <hyperlink ref="D6" r:id="rId11" location="gid=0" display="https://docs.google.com/spreadsheets/d/12DPrYeJiZaE2-wlKT0OwaTWSnyvkYB1vpcTBEgwJZhI/edit - gid=0" xr:uid="{AA90E64A-F243-4160-990F-7EB8B41CA9A6}"/>
+    <hyperlink ref="D45" r:id="rId12" xr:uid="{0BF29313-5C58-F84A-844C-469B17583F54}"/>
+    <hyperlink ref="D46" r:id="rId13" xr:uid="{308CF8E3-8263-B14E-887F-641FC41E397E}"/>
+    <hyperlink ref="D47" r:id="rId14" xr:uid="{DFA9CA38-CC10-9B45-82D5-8C4F17A44517}"/>
+    <hyperlink ref="D48" r:id="rId15" xr:uid="{E73EFE8B-84FD-2B4D-BFA6-4A01447F13DE}"/>
+    <hyperlink ref="D49" r:id="rId16" xr:uid="{7FD84F98-1D42-F64A-92A1-15751DA11F4B}"/>
+    <hyperlink ref="D50" r:id="rId17" xr:uid="{407EE9D1-B676-5845-B807-FF309CD21BCF}"/>
+    <hyperlink ref="D51" r:id="rId18" xr:uid="{5DD62BC8-9580-4D4B-AAA1-B5542914391B}"/>
+    <hyperlink ref="D52" r:id="rId19" xr:uid="{0E18C6A8-BBD9-1540-B47E-57FE2C36A7EB}"/>
+    <hyperlink ref="D53" r:id="rId20" xr:uid="{2E461D1B-F37D-C945-9CB0-5AB4542098E3}"/>
+    <hyperlink ref="D54" r:id="rId21" xr:uid="{033D11A4-26E8-1646-8512-2F966A562C24}"/>
+    <hyperlink ref="D55" r:id="rId22" xr:uid="{AEA1FE9E-D279-C74B-9A22-D370101FC0E8}"/>
+    <hyperlink ref="D56" r:id="rId23" xr:uid="{7D4C08A8-EE10-A44A-924F-E85957A8E92A}"/>
+    <hyperlink ref="D57" r:id="rId24" xr:uid="{9CB463B1-DF61-8646-9CA2-EF285C56DD95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>